<commit_message>
Fix typo of date
変換プログラムがエラーになっていたのもついでに修正。
エクセルファイルの「記入日時」は最下行に書く必要あり。
</commit_message>
<xml_diff>
--- a/data/data_convert/tochigi_covid19_data.xlsx
+++ b/data/data_convert/tochigi_covid19_data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/takahisa.sakurai/private/covid19/data/data_convert/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\y-ishida\src\covid19\data\data_convert\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86889697-F3A9-4D0D-AFEB-D6F4F5D7373A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5380" yWindow="1700" windowWidth="21600" windowHeight="13040" activeTab="2"/>
+    <workbookView xWindow="11625" yWindow="960" windowWidth="21600" windowHeight="13035" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="陽性患者数(patients_summary)" sheetId="1" r:id="rId1"/>
@@ -20,16 +21,13 @@
   <definedNames>
     <definedName name="Z_9B8DBD5B_9B80_478D_B810_F68E336A62D2_.wvu.FilterData" localSheetId="0" hidden="1">'陽性患者数(patients_summary)'!$A$2:$B$82</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <customWorkbookViews>
     <customWorkbookView name="フィルタ 1" guid="{9B8DBD5B-9B80-478D-B810-F68E336A62D2}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,6 +37,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -229,7 +230,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd\ h:mm"/>
@@ -681,8 +682,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:G99"/>
@@ -692,14 +693,14 @@
       <selection pane="bottomLeft" activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
-    <col min="5" max="5" width="34.5" customWidth="1"/>
-    <col min="7" max="7" width="31.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="34.42578125" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
@@ -711,7 +712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>5</v>
       </c>
@@ -723,7 +724,7 @@
       <c r="E2" s="18"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -739,7 +740,7 @@
       </c>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>43844</v>
       </c>
@@ -752,7 +753,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>43845</v>
       </c>
@@ -765,7 +766,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>43846</v>
       </c>
@@ -778,7 +779,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>43847</v>
       </c>
@@ -791,7 +792,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>43848</v>
       </c>
@@ -804,7 +805,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>43849</v>
       </c>
@@ -817,7 +818,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>43850</v>
       </c>
@@ -830,7 +831,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>43851</v>
       </c>
@@ -843,7 +844,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>43852</v>
       </c>
@@ -856,7 +857,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>43853</v>
       </c>
@@ -869,7 +870,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <v>43854</v>
       </c>
@@ -882,7 +883,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <v>43855</v>
       </c>
@@ -895,7 +896,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>43856</v>
       </c>
@@ -908,7 +909,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <v>43857</v>
       </c>
@@ -921,7 +922,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>43858</v>
       </c>
@@ -934,7 +935,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>43859</v>
       </c>
@@ -947,7 +948,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>43860</v>
       </c>
@@ -960,7 +961,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
         <v>43861</v>
       </c>
@@ -973,7 +974,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
         <v>43862</v>
       </c>
@@ -986,7 +987,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
         <v>43863</v>
       </c>
@@ -999,7 +1000,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
         <v>43864</v>
       </c>
@@ -1012,7 +1013,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
         <v>43865</v>
       </c>
@@ -1025,7 +1026,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
         <v>43866</v>
       </c>
@@ -1038,7 +1039,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
         <v>43867</v>
       </c>
@@ -1051,7 +1052,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
         <v>43868</v>
       </c>
@@ -1064,7 +1065,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="8">
         <v>43869</v>
       </c>
@@ -1077,7 +1078,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="8">
         <v>43870</v>
       </c>
@@ -1090,7 +1091,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="8">
         <v>43871</v>
       </c>
@@ -1103,7 +1104,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="8">
         <v>43872</v>
       </c>
@@ -1116,7 +1117,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="8">
         <v>43873</v>
       </c>
@@ -1129,7 +1130,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="8">
         <v>43874</v>
       </c>
@@ -1142,7 +1143,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="8">
         <v>43875</v>
       </c>
@@ -1155,7 +1156,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="8">
         <v>43876</v>
       </c>
@@ -1168,7 +1169,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="8">
         <v>43877</v>
       </c>
@@ -1181,7 +1182,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="8">
         <v>43878</v>
       </c>
@@ -1194,7 +1195,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="8">
         <v>43879</v>
       </c>
@@ -1207,7 +1208,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="8">
         <v>43880</v>
       </c>
@@ -1220,7 +1221,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="8">
         <v>43881</v>
       </c>
@@ -1233,7 +1234,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="8">
         <v>43882</v>
       </c>
@@ -1246,7 +1247,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="8">
         <v>43883</v>
       </c>
@@ -1261,7 +1262,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="8">
         <v>43884</v>
       </c>
@@ -1274,7 +1275,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="8">
         <v>43885</v>
       </c>
@@ -1287,7 +1288,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="8">
         <v>43886</v>
       </c>
@@ -1300,7 +1301,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="8">
         <v>43887</v>
       </c>
@@ -1313,7 +1314,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="8">
         <v>43888</v>
       </c>
@@ -1326,7 +1327,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="8">
         <v>43889</v>
       </c>
@@ -1339,7 +1340,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="8">
         <v>43890</v>
       </c>
@@ -1352,7 +1353,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="8">
         <v>43891</v>
       </c>
@@ -1365,7 +1366,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="8">
         <v>43892</v>
       </c>
@@ -1378,7 +1379,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="8">
         <v>43893</v>
       </c>
@@ -1391,7 +1392,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="8">
         <v>43894</v>
       </c>
@@ -1404,7 +1405,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="8">
         <v>43895</v>
       </c>
@@ -1419,7 +1420,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="8">
         <v>43896</v>
       </c>
@@ -1432,7 +1433,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="8">
         <v>43897</v>
       </c>
@@ -1445,7 +1446,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="8">
         <v>43898</v>
       </c>
@@ -1458,7 +1459,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="8">
         <v>43899</v>
       </c>
@@ -1471,7 +1472,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="8">
         <v>43900</v>
       </c>
@@ -1484,7 +1485,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="8">
         <v>43901</v>
       </c>
@@ -1497,7 +1498,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="8">
         <v>43902</v>
       </c>
@@ -1510,7 +1511,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="8">
         <v>43903</v>
       </c>
@@ -1523,7 +1524,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="8">
         <v>43904</v>
       </c>
@@ -1536,7 +1537,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="8">
         <v>43905</v>
       </c>
@@ -1549,7 +1550,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="8">
         <v>43906</v>
       </c>
@@ -1562,7 +1563,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="8">
         <v>43907</v>
       </c>
@@ -1575,7 +1576,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="8">
         <v>43908</v>
       </c>
@@ -1590,7 +1591,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="8">
         <v>43909</v>
       </c>
@@ -1603,7 +1604,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="8">
         <v>43910</v>
       </c>
@@ -1618,7 +1619,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="8">
         <v>43911</v>
       </c>
@@ -1631,7 +1632,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="8">
         <v>43912</v>
       </c>
@@ -1644,7 +1645,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="8">
         <v>43913</v>
       </c>
@@ -1657,7 +1658,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="8">
         <v>43914</v>
       </c>
@@ -1672,7 +1673,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="8">
         <v>43915</v>
       </c>
@@ -1687,7 +1688,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="8">
         <v>43916</v>
       </c>
@@ -1702,7 +1703,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="8">
         <v>43917</v>
       </c>
@@ -1715,7 +1716,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="8">
         <v>43918</v>
       </c>
@@ -1728,7 +1729,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="8">
         <v>43919</v>
       </c>
@@ -1743,7 +1744,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="8">
         <v>43921</v>
       </c>
@@ -1758,7 +1759,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="8">
         <v>43922</v>
       </c>
@@ -1773,7 +1774,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="8">
         <v>43923</v>
       </c>
@@ -1786,7 +1787,7 @@
       </c>
       <c r="E82" s="2"/>
     </row>
-    <row r="83" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="8">
         <v>43924</v>
       </c>
@@ -1798,7 +1799,7 @@
         <v>43928.965277777781</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="8">
         <v>43925</v>
       </c>
@@ -1811,7 +1812,7 @@
       </c>
       <c r="E84" s="2"/>
     </row>
-    <row r="85" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="8">
         <v>43926</v>
       </c>
@@ -1824,7 +1825,7 @@
       </c>
       <c r="E85" s="2"/>
     </row>
-    <row r="86" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="8">
         <v>43927</v>
       </c>
@@ -1839,7 +1840,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="91" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A87" s="8">
         <v>43928</v>
       </c>
@@ -1854,84 +1855,84 @@
         <v>53</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
     </row>
-    <row r="89" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
     </row>
-    <row r="90" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
     </row>
-    <row r="91" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
     </row>
-    <row r="92" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
     </row>
-    <row r="93" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
     </row>
-    <row r="94" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
     </row>
-    <row r="95" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
     </row>
-    <row r="96" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
     </row>
-    <row r="97" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
     </row>
-    <row r="98" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
     </row>
-    <row r="99" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -1942,7 +1943,7 @@
   <customSheetViews>
     <customSheetView guid="{9B8DBD5B-9B80-478D-B810-F68E336A62D2}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:B82"/>
+      <autoFilter ref="A2:B82" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="4">
@@ -1953,24 +1954,24 @@
   </mergeCells>
   <phoneticPr fontId="10"/>
   <hyperlinks>
-    <hyperlink ref="E43" r:id="rId1"/>
-    <hyperlink ref="E55" r:id="rId2"/>
-    <hyperlink ref="E68" r:id="rId3"/>
-    <hyperlink ref="E70" r:id="rId4"/>
-    <hyperlink ref="E74" r:id="rId5"/>
-    <hyperlink ref="E75" r:id="rId6"/>
-    <hyperlink ref="E76" r:id="rId7"/>
-    <hyperlink ref="E79" r:id="rId8"/>
-    <hyperlink ref="E80" r:id="rId9"/>
-    <hyperlink ref="E81" r:id="rId10"/>
+    <hyperlink ref="E43" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E55" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E68" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E70" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E74" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E75" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E76" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E79" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E80" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E81" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:J28"/>
@@ -1980,15 +1981,15 @@
       <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="83" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" customWidth="1"/>
-    <col min="9" max="9" width="84.83203125" customWidth="1"/>
-    <col min="10" max="10" width="31.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="84.85546875" customWidth="1"/>
+    <col min="10" max="10" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -2003,7 +2004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>6</v>
       </c>
@@ -2019,7 +2020,7 @@
       <c r="I2" s="18"/>
       <c r="J2" s="15"/>
     </row>
-    <row r="3" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -2047,7 +2048,7 @@
       </c>
       <c r="J3" s="15"/>
     </row>
-    <row r="4" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -2074,7 +2075,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -2101,7 +2102,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -2128,7 +2129,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -2155,7 +2156,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -2180,7 +2181,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -2205,7 +2206,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -2232,7 +2233,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -2257,7 +2258,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>9</v>
       </c>
@@ -2282,7 +2283,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -2307,7 +2308,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>11</v>
       </c>
@@ -2332,7 +2333,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>12</v>
       </c>
@@ -2357,7 +2358,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>13</v>
       </c>
@@ -2382,7 +2383,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="13" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>14</v>
       </c>
@@ -2407,7 +2408,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="13" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>15</v>
       </c>
@@ -2432,7 +2433,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>16</v>
       </c>
@@ -2457,7 +2458,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="13" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>17</v>
       </c>
@@ -2482,7 +2483,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>18</v>
       </c>
@@ -2507,7 +2508,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>19</v>
       </c>
@@ -2532,7 +2533,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>20</v>
       </c>
@@ -2557,7 +2558,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>21</v>
       </c>
@@ -2582,7 +2583,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>22</v>
       </c>
@@ -2607,7 +2608,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="13" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2618,7 +2619,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" ht="13" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2629,7 +2630,7 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" ht="13" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2649,50 +2650,50 @@
   </mergeCells>
   <phoneticPr fontId="10"/>
   <hyperlinks>
-    <hyperlink ref="I4" r:id="rId1"/>
-    <hyperlink ref="I5" r:id="rId2"/>
-    <hyperlink ref="I6" r:id="rId3"/>
-    <hyperlink ref="I7" r:id="rId4"/>
-    <hyperlink ref="I8" r:id="rId5"/>
-    <hyperlink ref="I9" r:id="rId6"/>
-    <hyperlink ref="I10" r:id="rId7"/>
-    <hyperlink ref="I11" r:id="rId8"/>
-    <hyperlink ref="I12" r:id="rId9"/>
-    <hyperlink ref="I13" r:id="rId10"/>
-    <hyperlink ref="I14" r:id="rId11"/>
-    <hyperlink ref="I15" r:id="rId12"/>
-    <hyperlink ref="I16" r:id="rId13"/>
-    <hyperlink ref="I17" r:id="rId14"/>
-    <hyperlink ref="I18" r:id="rId15"/>
-    <hyperlink ref="I19" r:id="rId16"/>
-    <hyperlink ref="I20" r:id="rId17"/>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="I5" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="I6" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="I7" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="I8" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="I9" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="I10" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="I11" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="I12" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="I13" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="I14" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="I15" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="I16" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="I17" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="I18" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="I19" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="I20" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:G95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F88" sqref="F88"/>
+      <selection pane="bottomLeft" activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
     <col min="6" max="6" width="83" customWidth="1"/>
-    <col min="7" max="7" width="31.6640625" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
@@ -2704,7 +2705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>7</v>
       </c>
@@ -2717,7 +2718,7 @@
       <c r="F2" s="18"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>11</v>
       </c>
@@ -2732,7 +2733,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="22"/>
       <c r="B4" s="10">
         <f t="shared" ref="B4:C4" si="0">SUM(B5:B95)</f>
@@ -2754,7 +2755,7 @@
       </c>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>43844</v>
       </c>
@@ -2771,7 +2772,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>43845</v>
       </c>
@@ -2788,7 +2789,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>43846</v>
       </c>
@@ -2805,7 +2806,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>43847</v>
       </c>
@@ -2822,7 +2823,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>43848</v>
       </c>
@@ -2839,7 +2840,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>43849</v>
       </c>
@@ -2856,7 +2857,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>43850</v>
       </c>
@@ -2873,7 +2874,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>43851</v>
       </c>
@@ -2890,7 +2891,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>43852</v>
       </c>
@@ -2907,7 +2908,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <v>43853</v>
       </c>
@@ -2924,7 +2925,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <v>43854</v>
       </c>
@@ -2941,7 +2942,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>43855</v>
       </c>
@@ -2958,7 +2959,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <v>43856</v>
       </c>
@@ -2975,7 +2976,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>43857</v>
       </c>
@@ -2992,7 +2993,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>43858</v>
       </c>
@@ -3009,7 +3010,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>43859</v>
       </c>
@@ -3026,7 +3027,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
         <v>43860</v>
       </c>
@@ -3043,7 +3044,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
         <v>43861</v>
       </c>
@@ -3060,7 +3061,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
         <v>43862</v>
       </c>
@@ -3077,7 +3078,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
         <v>43863</v>
       </c>
@@ -3094,7 +3095,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
         <v>43864</v>
       </c>
@@ -3111,7 +3112,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
         <v>43865</v>
       </c>
@@ -3128,7 +3129,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
         <v>43866</v>
       </c>
@@ -3145,7 +3146,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
         <v>43867</v>
       </c>
@@ -3162,7 +3163,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="8">
         <v>43868</v>
       </c>
@@ -3179,7 +3180,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="8">
         <v>43869</v>
       </c>
@@ -3196,7 +3197,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="8">
         <v>43870</v>
       </c>
@@ -3213,7 +3214,7 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="8">
         <v>43871</v>
       </c>
@@ -3230,7 +3231,7 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="8">
         <v>43872</v>
       </c>
@@ -3247,7 +3248,7 @@
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="8">
         <v>43873</v>
       </c>
@@ -3264,7 +3265,7 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="8">
         <v>43874</v>
       </c>
@@ -3281,7 +3282,7 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="8">
         <v>43875</v>
       </c>
@@ -3298,7 +3299,7 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="8">
         <v>43876</v>
       </c>
@@ -3315,7 +3316,7 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
     </row>
-    <row r="38" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="8">
         <v>43877</v>
       </c>
@@ -3332,7 +3333,7 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="8">
         <v>43878</v>
       </c>
@@ -3349,7 +3350,7 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
     </row>
-    <row r="40" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="8">
         <v>43879</v>
       </c>
@@ -3366,7 +3367,7 @@
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="8">
         <v>43880</v>
       </c>
@@ -3383,7 +3384,7 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="8">
         <v>43881</v>
       </c>
@@ -3400,7 +3401,7 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="8">
         <v>43882</v>
       </c>
@@ -3417,7 +3418,7 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="8">
         <v>43883</v>
       </c>
@@ -3434,7 +3435,7 @@
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="8">
         <v>43884</v>
       </c>
@@ -3451,7 +3452,7 @@
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
     </row>
-    <row r="46" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="8">
         <v>43885</v>
       </c>
@@ -3468,7 +3469,7 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
     </row>
-    <row r="47" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="8">
         <v>43886</v>
       </c>
@@ -3485,7 +3486,7 @@
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
     </row>
-    <row r="48" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="8">
         <v>43887</v>
       </c>
@@ -3502,7 +3503,7 @@
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="8">
         <v>43888</v>
       </c>
@@ -3519,7 +3520,7 @@
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
     </row>
-    <row r="50" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="8">
         <v>43889</v>
       </c>
@@ -3536,7 +3537,7 @@
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="8">
         <v>43890</v>
       </c>
@@ -3553,7 +3554,7 @@
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
     </row>
-    <row r="52" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="8">
         <v>43891</v>
       </c>
@@ -3570,7 +3571,7 @@
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
     </row>
-    <row r="53" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="8">
         <v>43892</v>
       </c>
@@ -3587,7 +3588,7 @@
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
     </row>
-    <row r="54" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="8">
         <v>43893</v>
       </c>
@@ -3604,7 +3605,7 @@
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
     </row>
-    <row r="55" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="8">
         <v>43894</v>
       </c>
@@ -3621,7 +3622,7 @@
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
     </row>
-    <row r="56" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="8">
         <v>43895</v>
       </c>
@@ -3638,7 +3639,7 @@
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
     </row>
-    <row r="57" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="8">
         <v>43896</v>
       </c>
@@ -3655,7 +3656,7 @@
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
     </row>
-    <row r="58" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="8">
         <v>43897</v>
       </c>
@@ -3672,7 +3673,7 @@
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
     </row>
-    <row r="59" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="8">
         <v>43898</v>
       </c>
@@ -3689,7 +3690,7 @@
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
     </row>
-    <row r="60" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="8">
         <v>43899</v>
       </c>
@@ -3706,7 +3707,7 @@
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
     </row>
-    <row r="61" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="8">
         <v>43900</v>
       </c>
@@ -3723,7 +3724,7 @@
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
     </row>
-    <row r="62" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="8">
         <v>43901</v>
       </c>
@@ -3740,7 +3741,7 @@
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
     </row>
-    <row r="63" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="8">
         <v>43902</v>
       </c>
@@ -3757,7 +3758,7 @@
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
     </row>
-    <row r="64" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="8">
         <v>43903</v>
       </c>
@@ -3774,7 +3775,7 @@
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
     </row>
-    <row r="65" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="8">
         <v>43904</v>
       </c>
@@ -3791,7 +3792,7 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
     </row>
-    <row r="66" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="8">
         <v>43905</v>
       </c>
@@ -3808,7 +3809,7 @@
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
     </row>
-    <row r="67" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="8">
         <v>43906</v>
       </c>
@@ -3825,7 +3826,7 @@
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
     </row>
-    <row r="68" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="8">
         <v>43907</v>
       </c>
@@ -3842,7 +3843,7 @@
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
     </row>
-    <row r="69" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="8">
         <v>43908</v>
       </c>
@@ -3859,7 +3860,7 @@
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="8">
         <v>43909</v>
       </c>
@@ -3880,7 +3881,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="8">
         <v>43910</v>
       </c>
@@ -3897,7 +3898,7 @@
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="8">
         <v>43911</v>
       </c>
@@ -3914,7 +3915,7 @@
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
     </row>
-    <row r="73" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="8">
         <v>43912</v>
       </c>
@@ -3931,7 +3932,7 @@
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
     </row>
-    <row r="74" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="8">
         <v>43913</v>
       </c>
@@ -3948,7 +3949,7 @@
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
     </row>
-    <row r="75" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="8">
         <v>43914</v>
       </c>
@@ -3965,7 +3966,7 @@
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
     </row>
-    <row r="76" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="8">
         <v>43915</v>
       </c>
@@ -3982,7 +3983,7 @@
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
     </row>
-    <row r="77" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="8">
         <v>43916</v>
       </c>
@@ -3999,7 +4000,7 @@
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
     </row>
-    <row r="78" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="8">
         <v>43917</v>
       </c>
@@ -4016,7 +4017,7 @@
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
     </row>
-    <row r="79" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="8">
         <v>43918</v>
       </c>
@@ -4033,7 +4034,7 @@
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
     </row>
-    <row r="80" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="8">
         <v>43919</v>
       </c>
@@ -4050,7 +4051,7 @@
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
     </row>
-    <row r="81" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="8">
         <v>43920</v>
       </c>
@@ -4067,7 +4068,7 @@
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
     </row>
-    <row r="82" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="8">
         <v>43921</v>
       </c>
@@ -4084,7 +4085,7 @@
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
     </row>
-    <row r="83" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="8">
         <v>43922</v>
       </c>
@@ -4105,7 +4106,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="8">
         <v>43923</v>
       </c>
@@ -4126,7 +4127,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="8">
         <v>43924</v>
       </c>
@@ -4139,14 +4140,10 @@
       <c r="D85" s="10">
         <v>44</v>
       </c>
-      <c r="E85" s="9">
-        <v>43929.98541666667</v>
-      </c>
-      <c r="F85" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="E85" s="9"/>
+      <c r="F85" s="11"/>
+    </row>
+    <row r="86" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="8">
         <v>43925</v>
       </c>
@@ -4162,7 +4159,7 @@
       <c r="E86" s="9"/>
       <c r="F86" s="11"/>
     </row>
-    <row r="87" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="8">
         <v>43926</v>
       </c>
@@ -4178,7 +4175,7 @@
       <c r="E87" s="9"/>
       <c r="F87" s="11"/>
     </row>
-    <row r="88" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="8">
         <v>43927</v>
       </c>
@@ -4191,10 +4188,14 @@
       <c r="D88" s="10">
         <v>25</v>
       </c>
-      <c r="E88" s="9"/>
-      <c r="F88" s="11"/>
-    </row>
-    <row r="89" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="E88" s="9">
+        <v>43929.98541666667</v>
+      </c>
+      <c r="F88" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="8"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
@@ -4205,7 +4206,7 @@
       <c r="E89" s="9"/>
       <c r="F89" s="11"/>
     </row>
-    <row r="90" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -4216,7 +4217,7 @@
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
     </row>
-    <row r="91" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -4227,7 +4228,7 @@
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
     </row>
-    <row r="92" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -4238,7 +4239,7 @@
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
     </row>
-    <row r="93" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -4249,7 +4250,7 @@
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
     </row>
-    <row r="94" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -4260,7 +4261,7 @@
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
     </row>
-    <row r="95" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -4281,34 +4282,34 @@
   </mergeCells>
   <phoneticPr fontId="10"/>
   <hyperlinks>
-    <hyperlink ref="F70" r:id="rId1"/>
-    <hyperlink ref="F83" r:id="rId2"/>
-    <hyperlink ref="F84" r:id="rId3"/>
+    <hyperlink ref="F70" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="F83" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="F84" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:F96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D82" sqref="D82"/>
+      <selection pane="bottomLeft" activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="31.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>47</v>
       </c>
@@ -4319,7 +4320,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>48</v>
       </c>
@@ -4331,7 +4332,7 @@
       <c r="E2" s="18"/>
       <c r="F2" s="15"/>
     </row>
-    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>11</v>
       </c>
@@ -4343,7 +4344,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="22"/>
       <c r="B4" s="10">
         <f>SUM(B5:B95)</f>
@@ -4358,7 +4359,7 @@
       </c>
       <c r="F4" s="15"/>
     </row>
-    <row r="5" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>43844</v>
       </c>
@@ -4369,7 +4370,7 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>43845</v>
       </c>
@@ -4380,7 +4381,7 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>43846</v>
       </c>
@@ -4391,7 +4392,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>43847</v>
       </c>
@@ -4402,7 +4403,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>43848</v>
       </c>
@@ -4413,7 +4414,7 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>43849</v>
       </c>
@@ -4424,7 +4425,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>43850</v>
       </c>
@@ -4435,7 +4436,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>43851</v>
       </c>
@@ -4446,7 +4447,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>43852</v>
       </c>
@@ -4457,7 +4458,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <v>43853</v>
       </c>
@@ -4468,7 +4469,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <v>43854</v>
       </c>
@@ -4479,7 +4480,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>43855</v>
       </c>
@@ -4490,7 +4491,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <v>43856</v>
       </c>
@@ -4501,7 +4502,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>43857</v>
       </c>
@@ -4512,7 +4513,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>43858</v>
       </c>
@@ -4523,7 +4524,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>43859</v>
       </c>
@@ -4534,7 +4535,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
         <v>43860</v>
       </c>
@@ -4545,7 +4546,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
         <v>43861</v>
       </c>
@@ -4556,7 +4557,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
         <v>43862</v>
       </c>
@@ -4567,7 +4568,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
         <v>43863</v>
       </c>
@@ -4578,7 +4579,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
         <v>43864</v>
       </c>
@@ -4589,7 +4590,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
         <v>43865</v>
       </c>
@@ -4600,7 +4601,7 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
         <v>43866</v>
       </c>
@@ -4611,7 +4612,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
         <v>43867</v>
       </c>
@@ -4622,7 +4623,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="8">
         <v>43868</v>
       </c>
@@ -4633,7 +4634,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="8">
         <v>43869</v>
       </c>
@@ -4644,7 +4645,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="8">
         <v>43870</v>
       </c>
@@ -4655,7 +4656,7 @@
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="8">
         <v>43871</v>
       </c>
@@ -4666,7 +4667,7 @@
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="8">
         <v>43872</v>
       </c>
@@ -4677,7 +4678,7 @@
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="8">
         <v>43873</v>
       </c>
@@ -4688,7 +4689,7 @@
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="8">
         <v>43874</v>
       </c>
@@ -4699,7 +4700,7 @@
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="8">
         <v>43875</v>
       </c>
@@ -4710,7 +4711,7 @@
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="8">
         <v>43876</v>
       </c>
@@ -4721,7 +4722,7 @@
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="8">
         <v>43877</v>
       </c>
@@ -4732,7 +4733,7 @@
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="8">
         <v>43878</v>
       </c>
@@ -4743,7 +4744,7 @@
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="8">
         <v>43879</v>
       </c>
@@ -4754,7 +4755,7 @@
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
     </row>
-    <row r="41" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="8">
         <v>43880</v>
       </c>
@@ -4765,7 +4766,7 @@
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
     </row>
-    <row r="42" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="8">
         <v>43881</v>
       </c>
@@ -4776,7 +4777,7 @@
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
     </row>
-    <row r="43" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="8">
         <v>43882</v>
       </c>
@@ -4787,7 +4788,7 @@
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
     </row>
-    <row r="44" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="8">
         <v>43883</v>
       </c>
@@ -4798,7 +4799,7 @@
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
     </row>
-    <row r="45" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="8">
         <v>43884</v>
       </c>
@@ -4809,7 +4810,7 @@
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
     </row>
-    <row r="46" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="8">
         <v>43885</v>
       </c>
@@ -4820,7 +4821,7 @@
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
     </row>
-    <row r="47" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="8">
         <v>43886</v>
       </c>
@@ -4831,7 +4832,7 @@
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
     </row>
-    <row r="48" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="8">
         <v>43887</v>
       </c>
@@ -4842,7 +4843,7 @@
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
     </row>
-    <row r="49" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="8">
         <v>43888</v>
       </c>
@@ -4853,7 +4854,7 @@
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
     </row>
-    <row r="50" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="8">
         <v>43889</v>
       </c>
@@ -4864,7 +4865,7 @@
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
     </row>
-    <row r="51" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="8">
         <v>43890</v>
       </c>
@@ -4875,7 +4876,7 @@
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
     </row>
-    <row r="52" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="8">
         <v>43891</v>
       </c>
@@ -4886,7 +4887,7 @@
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
     </row>
-    <row r="53" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="8">
         <v>43892</v>
       </c>
@@ -4897,7 +4898,7 @@
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
     </row>
-    <row r="54" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="8">
         <v>43893</v>
       </c>
@@ -4908,7 +4909,7 @@
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
     </row>
-    <row r="55" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="8">
         <v>43894</v>
       </c>
@@ -4919,7 +4920,7 @@
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
     </row>
-    <row r="56" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="8">
         <v>43895</v>
       </c>
@@ -4930,7 +4931,7 @@
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
     </row>
-    <row r="57" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="8">
         <v>43896</v>
       </c>
@@ -4941,7 +4942,7 @@
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
     </row>
-    <row r="58" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="8">
         <v>43897</v>
       </c>
@@ -4952,7 +4953,7 @@
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
     </row>
-    <row r="59" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="8">
         <v>43898</v>
       </c>
@@ -4963,7 +4964,7 @@
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
     </row>
-    <row r="60" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="8">
         <v>43899</v>
       </c>
@@ -4974,7 +4975,7 @@
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
     </row>
-    <row r="61" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="8">
         <v>43900</v>
       </c>
@@ -4985,7 +4986,7 @@
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
     </row>
-    <row r="62" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="8">
         <v>43901</v>
       </c>
@@ -4996,7 +4997,7 @@
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
     </row>
-    <row r="63" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="8">
         <v>43902</v>
       </c>
@@ -5007,7 +5008,7 @@
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
     </row>
-    <row r="64" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="8">
         <v>43903</v>
       </c>
@@ -5018,7 +5019,7 @@
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
     </row>
-    <row r="65" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="8">
         <v>43904</v>
       </c>
@@ -5029,7 +5030,7 @@
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
     </row>
-    <row r="66" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="8">
         <v>43905</v>
       </c>
@@ -5040,7 +5041,7 @@
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
     </row>
-    <row r="67" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="8">
         <v>43906</v>
       </c>
@@ -5051,7 +5052,7 @@
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
     </row>
-    <row r="68" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="8">
         <v>43907</v>
       </c>
@@ -5062,7 +5063,7 @@
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
     </row>
-    <row r="69" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="8">
         <v>43908</v>
       </c>
@@ -5077,7 +5078,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="8">
         <v>43909</v>
       </c>
@@ -5088,7 +5089,7 @@
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
     </row>
-    <row r="71" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="8">
         <v>43910</v>
       </c>
@@ -5099,7 +5100,7 @@
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
     </row>
-    <row r="72" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="8">
         <v>43911</v>
       </c>
@@ -5110,7 +5111,7 @@
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
     </row>
-    <row r="73" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="8">
         <v>43912</v>
       </c>
@@ -5121,7 +5122,7 @@
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
     </row>
-    <row r="74" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="8">
         <v>43913</v>
       </c>
@@ -5132,7 +5133,7 @@
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
     </row>
-    <row r="75" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="8">
         <v>43914</v>
       </c>
@@ -5143,7 +5144,7 @@
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
     </row>
-    <row r="76" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="8">
         <v>43915</v>
       </c>
@@ -5154,7 +5155,7 @@
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
     </row>
-    <row r="77" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="8">
         <v>43916</v>
       </c>
@@ -5169,7 +5170,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="8">
         <v>43917</v>
       </c>
@@ -5177,14 +5178,10 @@
         <v>370</v>
       </c>
       <c r="C78" s="2"/>
-      <c r="D78" s="9">
-        <v>43929.98333333333</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="D78" s="9"/>
+      <c r="E78" s="2"/>
+    </row>
+    <row r="79" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="8">
         <v>43918</v>
       </c>
@@ -5195,7 +5192,7 @@
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
     </row>
-    <row r="80" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="8">
         <v>43919</v>
       </c>
@@ -5206,7 +5203,7 @@
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
     </row>
-    <row r="81" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="8">
         <v>43920</v>
       </c>
@@ -5217,7 +5214,7 @@
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
     </row>
-    <row r="82" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="8">
         <v>43921</v>
       </c>
@@ -5228,7 +5225,7 @@
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
     </row>
-    <row r="83" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="8">
         <v>43922</v>
       </c>
@@ -5239,7 +5236,7 @@
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
     </row>
-    <row r="84" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="8">
         <v>43923</v>
       </c>
@@ -5247,87 +5244,91 @@
         <v>657</v>
       </c>
       <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
-    </row>
-    <row r="85" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="D84" s="9">
+        <v>43929.98333333333</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
     </row>
-    <row r="86" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
     </row>
-    <row r="87" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
     </row>
-    <row r="88" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
     </row>
-    <row r="89" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
     </row>
-    <row r="90" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
     </row>
-    <row r="91" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
     </row>
-    <row r="92" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
     </row>
-    <row r="93" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
     </row>
-    <row r="94" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
     </row>
-    <row r="95" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
     </row>
-    <row r="96" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -5344,8 +5345,8 @@
   </mergeCells>
   <phoneticPr fontId="10"/>
   <hyperlinks>
-    <hyperlink ref="E69" r:id="rId1"/>
-    <hyperlink ref="E77" r:id="rId2"/>
+    <hyperlink ref="E69" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="E77" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>

</xml_diff>